<commit_message>
Fixed integration issue with bug project
</commit_message>
<xml_diff>
--- a/Football Game.xlsx
+++ b/Football Game.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="10035"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>AQUA</t>
   </si>
@@ -133,13 +133,16 @@
     <t>Title Cased Event Name</t>
   </si>
   <si>
-    <t>East</t>
-  </si>
-  <si>
-    <t>All Stars</t>
-  </si>
-  <si>
-    <t>West</t>
+    <t>Brookwood</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>Parkview</t>
+  </si>
+  <si>
+    <t>Panthers</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,14 +579,14 @@
         <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F2" t="str">
         <f>B11 &amp; "Images\V_" &amp; E2 &amp; ".png"</f>
-        <v>D:\PlayOn! Sports\cold-steel-xp\Images\V_BURNT_ORANGE.png</v>
+        <v>D:\PlayOn! Sports\cold-steel-xp\Images\V_OLD_GOLD.png</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -597,17 +600,17 @@
         <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F3" t="str">
         <f>B11 &amp; "Images\H_" &amp; E3 &amp; ".png"</f>
-        <v>D:\PlayOn! Sports\cold-steel-xp\Images\H_MAROON.png</v>
+        <v>D:\PlayOn! Sports\cold-steel-xp\Images\H_PURPLE.png</v>
       </c>
       <c r="H3" t="s">
         <v>1</v>
@@ -749,8 +752,5 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="D3" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Continue preparations for TN ALL STAR
</commit_message>
<xml_diff>
--- a/Football Game.xlsx
+++ b/Football Game.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="10035"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E9" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,9 +547,9 @@
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="59.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="59.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -654,6 +654,10 @@
       <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="F7" t="str">
+        <f>B7 &amp; ", " &amp; B8</f>
+        <v>Cookeville, TN</v>
+      </c>
       <c r="H7" t="s">
         <v>5</v>
       </c>
@@ -670,11 +674,19 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f>B2 &amp; " " &amp; C2</f>
+        <v>Brookwood Broncos</v>
+      </c>
       <c r="H9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" t="str">
+        <f>B3 &amp; " " &amp; C3</f>
+        <v>Parkview Panthers</v>
+      </c>
       <c r="H10" t="s">
         <v>8</v>
       </c>
@@ -741,7 +753,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select a color for the scorebug" sqref="E2">
       <formula1>COLORS</formula1>

</xml_diff>